<commit_message>
rename test case code
</commit_message>
<xml_diff>
--- a/Test Scenario FinalProject - Web.xlsx
+++ b/Test Scenario FinalProject - Web.xlsx
@@ -154,9 +154,6 @@
     <t>10. Open Cart</t>
   </si>
   <si>
-    <t>AP_001</t>
-  </si>
-  <si>
     <t>Album, beanie, and belt should exist in cart</t>
   </si>
   <si>
@@ -172,31 +169,7 @@
     <t>Items should be removed</t>
   </si>
   <si>
-    <t>AP_002</t>
-  </si>
-  <si>
     <t>Login</t>
-  </si>
-  <si>
-    <t>AP_003</t>
-  </si>
-  <si>
-    <t>AP_004</t>
-  </si>
-  <si>
-    <t>AP_005</t>
-  </si>
-  <si>
-    <t>AP_006</t>
-  </si>
-  <si>
-    <t>AP_007</t>
-  </si>
-  <si>
-    <t>AP_008</t>
-  </si>
-  <si>
-    <t>AP_009</t>
   </si>
   <si>
     <t>Login - Blank</t>
@@ -315,6 +288,33 @@
   </si>
   <si>
     <t>Returned polo items</t>
+  </si>
+  <si>
+    <t>WE_001</t>
+  </si>
+  <si>
+    <t>WE_002</t>
+  </si>
+  <si>
+    <t>WE_003</t>
+  </si>
+  <si>
+    <t>WE_004</t>
+  </si>
+  <si>
+    <t>WE_005</t>
+  </si>
+  <si>
+    <t>WE_006</t>
+  </si>
+  <si>
+    <t>WE_007</t>
+  </si>
+  <si>
+    <t>WE_008</t>
+  </si>
+  <si>
+    <t>WE_009</t>
   </si>
 </sst>
 </file>
@@ -684,6 +684,94 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -701,11 +789,13 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -714,96 +804,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB971"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45:F47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1043,22 +1043,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="51"/>
       <c r="C1" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22" t="s">
+      <c r="F1" s="51"/>
+      <c r="G1" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="53"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1111,22 +1111,22 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="26">
+      <c r="F3" s="51"/>
+      <c r="G3" s="56">
         <v>44754</v>
       </c>
-      <c r="H3" s="23"/>
+      <c r="H3" s="53"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1179,15 +1179,15 @@
       <c r="AB4" s="3"/>
     </row>
     <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="60" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1225,7 +1225,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="31"/>
+      <c r="E6" s="61"/>
       <c r="F6" s="10">
         <v>9</v>
       </c>
@@ -1290,16 +1290,16 @@
       <c r="A8" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="33"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="17" t="s">
         <v>13</v>
       </c>
@@ -1333,20 +1333,20 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="56" t="s">
+      <c r="A9" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="40" t="s">
+      <c r="E9" s="47"/>
+      <c r="F9" s="34" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="15" t="s">
@@ -1355,7 +1355,7 @@
       <c r="H9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="34" t="s">
         <v>6</v>
       </c>
       <c r="J9" s="2"/>
@@ -1379,21 +1379,21 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="47"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="27" t="s">
+      <c r="A10" s="43"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="41"/>
+      <c r="I10" s="35"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -1415,17 +1415,17 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="47"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="27" t="s">
+      <c r="A11" s="43"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
-      <c r="I11" s="41"/>
+      <c r="I11" s="35"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -1447,17 +1447,17 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="47"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="27" t="s">
+      <c r="A12" s="43"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="41"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
-      <c r="I12" s="41"/>
+      <c r="I12" s="35"/>
       <c r="J12" s="2"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -1479,21 +1479,21 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="47"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="39" t="s">
+      <c r="A13" s="43"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="41"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="41"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="2"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1515,21 +1515,21 @@
       <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="47"/>
-      <c r="B14" s="56"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="39" t="s">
+      <c r="A14" s="43"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="41"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="19" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="41"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="2"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -1551,17 +1551,17 @@
       <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="47"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="58" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="41"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="35"/>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
-      <c r="I15" s="41"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="2"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -1583,21 +1583,21 @@
       <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="47"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="58" t="s">
+      <c r="A16" s="43"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="41"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="19" t="s">
         <v>38</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="41"/>
+      <c r="I16" s="35"/>
       <c r="J16" s="2"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -1619,21 +1619,21 @@
       <c r="AB16" s="3"/>
     </row>
     <row r="17" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="47"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="58" t="s">
+      <c r="A17" s="43"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="59"/>
-      <c r="F17" s="41"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="19" t="s">
         <v>41</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="41"/>
+      <c r="I17" s="35"/>
       <c r="J17" s="2"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
@@ -1655,21 +1655,21 @@
       <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="48"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="58" t="s">
+      <c r="A18" s="44"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="42"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="42"/>
+      <c r="I18" s="36"/>
       <c r="J18" s="2"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -1691,19 +1691,19 @@
       <c r="AB18" s="3"/>
     </row>
     <row r="19" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="56"/>
-      <c r="C19" s="40" t="s">
+      <c r="A19" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" s="22"/>
+      <c r="C19" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="61"/>
-      <c r="F19" s="40" t="s">
-        <v>65</v>
+      <c r="E19" s="59"/>
+      <c r="F19" s="34" t="s">
+        <v>56</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>17</v>
@@ -1711,7 +1711,7 @@
       <c r="H19" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I19" s="52" t="s">
+      <c r="I19" s="24" t="s">
         <v>6</v>
       </c>
       <c r="J19" s="4"/>
@@ -1735,21 +1735,21 @@
       <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="56"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="60" t="s">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="41"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="53"/>
+      <c r="I20" s="25"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -1771,17 +1771,17 @@
       <c r="AB20" s="3"/>
     </row>
     <row r="21" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="56"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="60" t="s">
+      <c r="A21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="61"/>
-      <c r="F21" s="41"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
-      <c r="I21" s="53"/>
+      <c r="I21" s="25"/>
       <c r="J21" s="4"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1803,17 +1803,17 @@
       <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="56"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="60" t="s">
+      <c r="A22" s="22"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="61"/>
-      <c r="F22" s="41"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
-      <c r="I22" s="53"/>
+      <c r="I22" s="25"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1835,21 +1835,21 @@
       <c r="AB22" s="3"/>
     </row>
     <row r="23" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="56"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="58" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="41"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="53"/>
+      <c r="I23" s="25"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
@@ -1871,21 +1871,21 @@
       <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="56"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="58" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="59"/>
-      <c r="F24" s="41"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="35"/>
       <c r="G24" s="19" t="s">
         <v>35</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="53"/>
+      <c r="I24" s="25"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
@@ -1907,17 +1907,17 @@
       <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="56"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="58" t="s">
+      <c r="A25" s="22"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="59"/>
-      <c r="F25" s="41"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="35"/>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
-      <c r="I25" s="53"/>
+      <c r="I25" s="25"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1939,21 +1939,21 @@
       <c r="AB25" s="3"/>
     </row>
     <row r="26" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="56"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="58" t="s">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="59"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="35"/>
       <c r="G26" s="19" t="s">
         <v>38</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="25"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1975,21 +1975,21 @@
       <c r="AB26" s="3"/>
     </row>
     <row r="27" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="56"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="58" t="s">
+      <c r="A27" s="22"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="59"/>
-      <c r="F27" s="41"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="35"/>
       <c r="G27" s="19" t="s">
         <v>41</v>
       </c>
       <c r="H27" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I27" s="53"/>
+      <c r="I27" s="25"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -2011,21 +2011,21 @@
       <c r="AB27" s="3"/>
     </row>
     <row r="28" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="56"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="58" t="s">
+      <c r="A28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="59"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="35"/>
       <c r="G28" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H28" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="53"/>
+      <c r="I28" s="25"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -2047,21 +2047,21 @@
       <c r="AB28" s="3"/>
     </row>
     <row r="29" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="57"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="58" t="s">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="59"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="I29" s="54"/>
+      <c r="I29" s="26"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
@@ -2083,21 +2083,21 @@
       <c r="AB29" s="3"/>
     </row>
     <row r="30" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="27" t="s">
+      <c r="A30" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="40" t="s">
-        <v>64</v>
+      <c r="E30" s="47"/>
+      <c r="F30" s="34" t="s">
+        <v>55</v>
       </c>
       <c r="G30" s="15" t="s">
         <v>17</v>
@@ -2105,7 +2105,7 @@
       <c r="H30" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I30" s="52" t="s">
+      <c r="I30" s="24" t="s">
         <v>6</v>
       </c>
       <c r="J30" s="3"/>
@@ -2129,21 +2129,21 @@
       <c r="AB30" s="3"/>
     </row>
     <row r="31" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="56"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="27" t="s">
+      <c r="A31" s="22"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="41"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H31" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I31" s="53"/>
+      <c r="I31" s="25"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -2165,21 +2165,21 @@
       <c r="AB31" s="3"/>
     </row>
     <row r="32" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="57"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="28"/>
-      <c r="F32" s="42"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="47"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="19" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="I32" s="54"/>
+        <v>61</v>
+      </c>
+      <c r="I32" s="26"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -2201,19 +2201,19 @@
       <c r="AB32" s="3"/>
     </row>
     <row r="33" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="27" t="s">
+      <c r="A33" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="28"/>
+      <c r="C33" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="40" t="s">
-        <v>66</v>
+      <c r="E33" s="47"/>
+      <c r="F33" s="34" t="s">
+        <v>57</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>17</v>
@@ -2221,7 +2221,7 @@
       <c r="H33" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I33" s="43" t="s">
+      <c r="I33" s="27" t="s">
         <v>6</v>
       </c>
       <c r="J33" s="3"/>
@@ -2245,21 +2245,21 @@
       <c r="AB33" s="3"/>
     </row>
     <row r="34" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="47"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="27" t="s">
+      <c r="A34" s="43"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="28"/>
-      <c r="F34" s="41"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H34" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="44"/>
+      <c r="I34" s="28"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
@@ -2281,21 +2281,21 @@
       <c r="AB34" s="3"/>
     </row>
     <row r="35" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="42"/>
+      <c r="A35" s="44"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="47"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="I35" s="45"/>
+        <v>64</v>
+      </c>
+      <c r="I35" s="29"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -2317,19 +2317,19 @@
       <c r="AB35" s="3"/>
     </row>
     <row r="36" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="27" t="s">
+      <c r="A36" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="28"/>
+      <c r="C36" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="49" t="s">
-        <v>67</v>
+      <c r="E36" s="47"/>
+      <c r="F36" s="39" t="s">
+        <v>58</v>
       </c>
       <c r="G36" s="15" t="s">
         <v>17</v>
@@ -2337,7 +2337,7 @@
       <c r="H36" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I36" s="43" t="s">
+      <c r="I36" s="27" t="s">
         <v>6</v>
       </c>
       <c r="J36" s="3"/>
@@ -2361,21 +2361,21 @@
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="47"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="27" t="s">
+      <c r="A37" s="43"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="50"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H37" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="44"/>
+      <c r="I37" s="28"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -2397,21 +2397,21 @@
       <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="48"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="51"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="47"/>
+      <c r="F38" s="41"/>
       <c r="G38" s="19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="I38" s="44"/>
+        <v>64</v>
+      </c>
+      <c r="I38" s="28"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -2433,19 +2433,19 @@
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="27" t="s">
+      <c r="A39" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E39" s="28"/>
-      <c r="F39" s="49" t="s">
-        <v>68</v>
+      <c r="E39" s="47"/>
+      <c r="F39" s="39" t="s">
+        <v>59</v>
       </c>
       <c r="G39" s="15" t="s">
         <v>17</v>
@@ -2453,7 +2453,7 @@
       <c r="H39" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I39" s="43" t="s">
+      <c r="I39" s="27" t="s">
         <v>6</v>
       </c>
       <c r="J39" s="3"/>
@@ -2477,21 +2477,21 @@
       <c r="AB39" s="3"/>
     </row>
     <row r="40" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="47"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="27" t="s">
+      <c r="A40" s="43"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E40" s="28"/>
-      <c r="F40" s="50"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="40"/>
       <c r="G40" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H40" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="44"/>
+      <c r="I40" s="28"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -2513,21 +2513,21 @@
       <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="48"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="28"/>
-      <c r="F41" s="51"/>
+      <c r="A41" s="44"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="47"/>
+      <c r="F41" s="41"/>
       <c r="G41" s="19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H41" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="I41" s="44"/>
+        <v>64</v>
+      </c>
+      <c r="I41" s="28"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
@@ -2549,19 +2549,19 @@
       <c r="AB41" s="3"/>
     </row>
     <row r="42" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="47"/>
+      <c r="F42" s="39" t="s">
         <v>56</v>
-      </c>
-      <c r="B42" s="44"/>
-      <c r="C42" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="28"/>
-      <c r="F42" s="49" t="s">
-        <v>65</v>
       </c>
       <c r="G42" s="15" t="s">
         <v>17</v>
@@ -2569,7 +2569,7 @@
       <c r="H42" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I42" s="43" t="s">
+      <c r="I42" s="27" t="s">
         <v>6</v>
       </c>
       <c r="J42" s="3"/>
@@ -2593,21 +2593,21 @@
       <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="47"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="27" t="s">
+      <c r="A43" s="43"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="28"/>
-      <c r="F43" s="50"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="40"/>
       <c r="G43" s="19" t="s">
         <v>30</v>
       </c>
       <c r="H43" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I43" s="44"/>
+      <c r="I43" s="28"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -2629,21 +2629,21 @@
       <c r="AB43" s="3"/>
     </row>
     <row r="44" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
-      <c r="B44" s="45"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44" s="28"/>
-      <c r="F44" s="51"/>
+      <c r="A44" s="44"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="47"/>
+      <c r="F44" s="41"/>
       <c r="G44" s="19" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="I44" s="45"/>
+        <v>66</v>
+      </c>
+      <c r="I44" s="29"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
@@ -2665,21 +2665,21 @@
       <c r="AB44" s="3"/>
     </row>
     <row r="45" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="27" t="s">
+      <c r="A45" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="63" t="s">
-        <v>81</v>
+      <c r="E45" s="47"/>
+      <c r="F45" s="45" t="s">
+        <v>72</v>
       </c>
       <c r="G45" s="15" t="s">
         <v>17</v>
@@ -2687,7 +2687,7 @@
       <c r="H45" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I45" s="35" t="s">
+      <c r="I45" s="30" t="s">
         <v>6</v>
       </c>
       <c r="J45" s="3"/>
@@ -2711,21 +2711,21 @@
       <c r="AB45" s="3"/>
     </row>
     <row r="46" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="37"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="63"/>
+      <c r="A46" s="31"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="47"/>
+      <c r="F46" s="45"/>
       <c r="G46" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="I46" s="35"/>
+        <v>76</v>
+      </c>
+      <c r="I46" s="30"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
@@ -2747,21 +2747,21 @@
       <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="37"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E47" s="28"/>
-      <c r="F47" s="63"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47" s="47"/>
+      <c r="F47" s="45"/>
       <c r="G47" s="19" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="I47" s="35"/>
+        <v>75</v>
+      </c>
+      <c r="I47" s="30"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
@@ -2783,19 +2783,19 @@
       <c r="AB47" s="3"/>
     </row>
     <row r="48" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="D48" s="27" t="s">
+      <c r="A48" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="30"/>
+      <c r="C48" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E48" s="28"/>
-      <c r="F48" s="34" t="s">
-        <v>89</v>
+      <c r="E48" s="47"/>
+      <c r="F48" s="33" t="s">
+        <v>80</v>
       </c>
       <c r="G48" s="15" t="s">
         <v>17</v>
@@ -2803,7 +2803,7 @@
       <c r="H48" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="I48" s="35" t="s">
+      <c r="I48" s="30" t="s">
         <v>6</v>
       </c>
       <c r="J48" s="3"/>
@@ -2827,21 +2827,21 @@
       <c r="AB48" s="3"/>
     </row>
     <row r="49" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="37"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="E49" s="28"/>
-      <c r="F49" s="34"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="47"/>
+      <c r="F49" s="33"/>
       <c r="G49" s="19" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="I49" s="35"/>
+        <v>76</v>
+      </c>
+      <c r="I49" s="30"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
@@ -2863,21 +2863,21 @@
       <c r="AB49" s="3"/>
     </row>
     <row r="50" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="37"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="E50" s="28"/>
-      <c r="F50" s="34"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="47"/>
+      <c r="F50" s="33"/>
       <c r="G50" s="19" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="H50" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="I50" s="35"/>
+        <v>84</v>
+      </c>
+      <c r="I50" s="30"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
@@ -2899,21 +2899,21 @@
       <c r="AB50" s="3"/>
     </row>
     <row r="51" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="37"/>
-      <c r="B51" s="35"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="34"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="48"/>
+      <c r="F51" s="33"/>
       <c r="G51" s="19" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H51" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="I51" s="35"/>
+        <v>85</v>
+      </c>
+      <c r="I51" s="30"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
@@ -2935,21 +2935,21 @@
       <c r="AB51" s="3"/>
     </row>
     <row r="52" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="37"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="E52" s="36"/>
-      <c r="F52" s="34"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="48"/>
+      <c r="F52" s="33"/>
       <c r="G52" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="H52" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="I52" s="35"/>
+        <v>86</v>
+      </c>
+      <c r="I52" s="30"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
@@ -7922,6 +7922,82 @@
     <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="92">
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A9:A18"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="I36:I38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="I45:I47"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="C19:C29"/>
+    <mergeCell ref="F19:F29"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D23:E23"/>
     <mergeCell ref="A19:A29"/>
     <mergeCell ref="I19:I29"/>
     <mergeCell ref="B9:B29"/>
@@ -7938,82 +8014,6 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="C19:C29"/>
-    <mergeCell ref="F19:F29"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="I45:I47"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="I36:I38"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A9:A18"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>